<commit_message>
Done updating the new model
Done updating the new model, completed the quatrefoil and imported all into Unity, all that's left is to apply materials, textures and colliders then it's done
</commit_message>
<xml_diff>
--- a/Blender/Shape Dimensions.xlsx
+++ b/Blender/Shape Dimensions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin_faruq\OneDrive - York University\Desktop\Unity3D\VRMultiplayer(Normcore)\Blender\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A54EFB7C-D894-4340-865C-12E7CD744943}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78247496-FBDC-4FD7-BC76-72AB1AD0DF89}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="23235" windowHeight="14595" xr2:uid="{F8D9BBB8-DF6E-4383-B342-E7D00C59515B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="110">
   <si>
     <t>Shape</t>
   </si>
@@ -345,13 +345,16 @@
     <t>0.001185 m</t>
   </si>
   <si>
-    <t>semi circle rad</t>
-  </si>
-  <si>
     <t>semi circle extrude</t>
   </si>
   <si>
     <t>longer width</t>
+  </si>
+  <si>
+    <t>semi circle diameter</t>
+  </si>
+  <si>
+    <t>inner square</t>
   </si>
 </sst>
 </file>
@@ -375,7 +378,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -385,12 +388,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -407,11 +404,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -726,16 +722,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5C96A0B-6EA0-4CBE-8C48-8E546039F290}">
-  <dimension ref="A1:R77"/>
+  <dimension ref="A1:R78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="G75" sqref="G75"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.7109375" customWidth="1"/>
@@ -1096,7 +1092,7 @@
         <v>38.57</v>
       </c>
       <c r="K10">
-        <f t="shared" si="4"/>
+        <f>J10/1000</f>
         <v>3.857E-2</v>
       </c>
       <c r="L10" s="2"/>
@@ -1589,7 +1585,7 @@
         <f t="shared" si="2"/>
         <v>0.14008999999999999</v>
       </c>
-      <c r="L26" s="3"/>
+      <c r="L26" s="2"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
@@ -1616,7 +1612,7 @@
         <f>F27/1000</f>
         <v>0.13288999999999998</v>
       </c>
-      <c r="L27" s="3"/>
+      <c r="L27" s="2"/>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
@@ -2270,7 +2266,7 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C75">
         <v>18.399999999999999</v>
@@ -2279,10 +2275,18 @@
         <f>C75/1000</f>
         <v>1.84E-2</v>
       </c>
+      <c r="E75">
+        <f>D75*2</f>
+        <v>3.6799999999999999E-2</v>
+      </c>
+      <c r="F75">
+        <f>D75/2</f>
+        <v>9.1999999999999998E-3</v>
+      </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C76">
         <v>1.88</v>
@@ -2294,7 +2298,7 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C77">
         <v>44.26</v>
@@ -2302,6 +2306,23 @@
       <c r="D77">
         <f>C77/1000</f>
         <v>4.4260000000000001E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B78" t="s">
+        <v>109</v>
+      </c>
+      <c r="C78">
+        <f>C77-(C75+C76+C76)</f>
+        <v>22.1</v>
+      </c>
+      <c r="D78">
+        <f>C78/1000</f>
+        <v>2.2100000000000002E-2</v>
+      </c>
+      <c r="E78">
+        <f>D78/2</f>
+        <v>1.1050000000000001E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>